<commit_message>
here is the updated movie data.
sorry i could only add 30. I am really tired after work and feel myself falling asleep
</commit_message>
<xml_diff>
--- a/MovieData.xlsx
+++ b/MovieData.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2CD8FA-6987-4744-9C26-BEC6C2553703}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17820" yWindow="3450" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17820" yWindow="3456" windowWidth="21600" windowHeight="11388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Budget</t>
   </si>
@@ -97,12 +91,102 @@
   </si>
   <si>
     <t>Worldwide Gross</t>
+  </si>
+  <si>
+    <t>THE LITTLE MERMAID</t>
+  </si>
+  <si>
+    <t>HERCULES</t>
+  </si>
+  <si>
+    <t>THE NIGHTMARE BEFORE CHRISTMAS</t>
+  </si>
+  <si>
+    <t>ALADDIN</t>
+  </si>
+  <si>
+    <t>THE LION KING</t>
+  </si>
+  <si>
+    <t>ATLANTIS - DISNEY</t>
+  </si>
+  <si>
+    <t>TREASURE PLANET</t>
+  </si>
+  <si>
+    <t>THE IRON GIANT</t>
+  </si>
+  <si>
+    <t>THE JUNGLE BOOK</t>
+  </si>
+  <si>
+    <t>THE JUNGLE BOOK 2</t>
+  </si>
+  <si>
+    <t>POCAHONTAS</t>
+  </si>
+  <si>
+    <t>TOY STORY</t>
+  </si>
+  <si>
+    <t>TOY STORY 2</t>
+  </si>
+  <si>
+    <t>TOY STORY 3</t>
+  </si>
+  <si>
+    <t>THE HUNCHBACK OF NOTRE DAME</t>
+  </si>
+  <si>
+    <t>MULAN</t>
+  </si>
+  <si>
+    <t>A BUG'S LIFE</t>
+  </si>
+  <si>
+    <t>TARZAN</t>
+  </si>
+  <si>
+    <t>DINOSAUR</t>
+  </si>
+  <si>
+    <t>101 DALMATIANS</t>
+  </si>
+  <si>
+    <t>THE EMPEROR'S NEW GROOVE</t>
+  </si>
+  <si>
+    <t>MONSTERS, INC.</t>
+  </si>
+  <si>
+    <t>RETURN TO NEVER LAND</t>
+  </si>
+  <si>
+    <t>LILO &amp; STITCH</t>
+  </si>
+  <si>
+    <t>FINDING NEMO</t>
+  </si>
+  <si>
+    <t>FINDING DORY</t>
+  </si>
+  <si>
+    <t>BROTHER BEAR</t>
+  </si>
+  <si>
+    <t>THE INCREDIBLES</t>
+  </si>
+  <si>
+    <t>THE INCREDIBLES 2</t>
+  </si>
+  <si>
+    <t>NATIONAL TREASURE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,30 +514,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -946,6 +1030,876 @@
         <v>22</v>
       </c>
     </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>111543479</v>
+      </c>
+      <c r="B18" s="3">
+        <v>6031914</v>
+      </c>
+      <c r="C18" s="3">
+        <v>274176364</v>
+      </c>
+      <c r="D18" s="3">
+        <v>40000000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>88</v>
+      </c>
+      <c r="F18" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="G18" s="3">
+        <v>93</v>
+      </c>
+      <c r="H18" s="3">
+        <v>88</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>99112101</v>
+      </c>
+      <c r="B19" s="3">
+        <v>249567</v>
+      </c>
+      <c r="C19" s="3">
+        <v>252712101</v>
+      </c>
+      <c r="D19" s="3">
+        <v>85000000</v>
+      </c>
+      <c r="E19">
+        <v>74</v>
+      </c>
+      <c r="F19">
+        <v>7.3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>83</v>
+      </c>
+      <c r="H19" s="3">
+        <v>75</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>75085668</v>
+      </c>
+      <c r="B20" s="3">
+        <v>88850032</v>
+      </c>
+      <c r="C20" s="3">
+        <v>191232</v>
+      </c>
+      <c r="D20" s="3">
+        <v>18000000</v>
+      </c>
+      <c r="E20" s="3">
+        <v>82</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3">
+        <v>95</v>
+      </c>
+      <c r="H20" s="3">
+        <v>91</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>217350219</v>
+      </c>
+      <c r="B21" s="3">
+        <v>196664</v>
+      </c>
+      <c r="C21" s="3">
+        <v>504050219</v>
+      </c>
+      <c r="D21" s="3">
+        <v>28000000</v>
+      </c>
+      <c r="E21">
+        <v>86</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3">
+        <v>94</v>
+      </c>
+      <c r="H21" s="3">
+        <v>92</v>
+      </c>
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>422783777</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1586753</v>
+      </c>
+      <c r="C22" s="3">
+        <v>968511805</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45000000</v>
+      </c>
+      <c r="E22" s="3">
+        <v>83</v>
+      </c>
+      <c r="F22" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>93</v>
+      </c>
+      <c r="H22" s="3">
+        <v>93</v>
+      </c>
+      <c r="I22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>84056472</v>
+      </c>
+      <c r="B23" s="3">
+        <v>329011</v>
+      </c>
+      <c r="C23" s="3">
+        <v>186053725</v>
+      </c>
+      <c r="D23" s="3">
+        <v>120000000</v>
+      </c>
+      <c r="E23">
+        <v>52</v>
+      </c>
+      <c r="F23">
+        <v>6.9</v>
+      </c>
+      <c r="G23" s="3">
+        <v>49</v>
+      </c>
+      <c r="H23" s="3">
+        <v>53</v>
+      </c>
+      <c r="I23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>38176783</v>
+      </c>
+      <c r="B24" s="3">
+        <v>12083248</v>
+      </c>
+      <c r="C24" s="3">
+        <v>110041363</v>
+      </c>
+      <c r="D24" s="3">
+        <v>140000000</v>
+      </c>
+      <c r="E24" s="3">
+        <v>60</v>
+      </c>
+      <c r="F24" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="G24" s="3">
+        <v>69</v>
+      </c>
+      <c r="H24" s="3">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>23159305</v>
+      </c>
+      <c r="B25" s="3">
+        <v>5732614</v>
+      </c>
+      <c r="C25" s="3">
+        <v>23179225</v>
+      </c>
+      <c r="D25" s="3">
+        <v>70000000</v>
+      </c>
+      <c r="E25">
+        <v>85</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25" s="3">
+        <v>96</v>
+      </c>
+      <c r="H25" s="3">
+        <v>90</v>
+      </c>
+      <c r="I25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>141843612</v>
+      </c>
+      <c r="B26" s="3">
+        <v>5291670</v>
+      </c>
+      <c r="C26" s="3">
+        <v>210310084</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="E26" s="3">
+        <v>65</v>
+      </c>
+      <c r="F26" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="G26" s="3">
+        <v>87</v>
+      </c>
+      <c r="H26" s="3">
+        <v>82</v>
+      </c>
+      <c r="I26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>47901582</v>
+      </c>
+      <c r="B27" s="3">
+        <v>11441733</v>
+      </c>
+      <c r="C27" s="3">
+        <v>186307412</v>
+      </c>
+      <c r="D27" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="E27">
+        <v>38</v>
+      </c>
+      <c r="F27">
+        <v>5.4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>19</v>
+      </c>
+      <c r="H27" s="3">
+        <v>29</v>
+      </c>
+      <c r="I27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>141579773</v>
+      </c>
+      <c r="B28" s="3">
+        <v>2689714</v>
+      </c>
+      <c r="C28" s="3">
+        <v>346079773</v>
+      </c>
+      <c r="D28" s="3">
+        <v>55000000</v>
+      </c>
+      <c r="E28" s="3">
+        <v>58</v>
+      </c>
+      <c r="F28" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="G28" s="3">
+        <v>57</v>
+      </c>
+      <c r="H28" s="3">
+        <v>64</v>
+      </c>
+      <c r="I28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>222498679</v>
+      </c>
+      <c r="B29" s="3">
+        <v>29140617</v>
+      </c>
+      <c r="C29" s="3">
+        <v>415674866</v>
+      </c>
+      <c r="D29" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="E29">
+        <v>95</v>
+      </c>
+      <c r="F29">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G29" s="3">
+        <v>100</v>
+      </c>
+      <c r="H29" s="3">
+        <v>92</v>
+      </c>
+      <c r="I29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>242852179</v>
+      </c>
+      <c r="B30" s="3">
+        <v>300163</v>
+      </c>
+      <c r="C30" s="3">
+        <v>508793269</v>
+      </c>
+      <c r="D30" s="3">
+        <v>90000000</v>
+      </c>
+      <c r="E30" s="3">
+        <v>88</v>
+      </c>
+      <c r="F30" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="G30" s="3">
+        <v>100</v>
+      </c>
+      <c r="H30" s="3">
+        <v>86</v>
+      </c>
+      <c r="I30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>415004880</v>
+      </c>
+      <c r="B31" s="3">
+        <v>110307189</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1066969703</v>
+      </c>
+      <c r="D31" s="3">
+        <v>200000000</v>
+      </c>
+      <c r="E31">
+        <v>92</v>
+      </c>
+      <c r="F31">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G31" s="3">
+        <v>98</v>
+      </c>
+      <c r="H31" s="3">
+        <v>89</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>100138851</v>
+      </c>
+      <c r="B32" s="3">
+        <v>21037414</v>
+      </c>
+      <c r="C32" s="3">
+        <v>325338851</v>
+      </c>
+      <c r="D32" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="E32" s="3">
+        <v>74</v>
+      </c>
+      <c r="F32" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="G32" s="3">
+        <v>72</v>
+      </c>
+      <c r="H32" s="3">
+        <v>70</v>
+      </c>
+      <c r="I32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>120620254</v>
+      </c>
+      <c r="B33" s="3">
+        <v>22745143</v>
+      </c>
+      <c r="C33" s="3">
+        <v>304320254</v>
+      </c>
+      <c r="D33" s="3">
+        <v>90000000</v>
+      </c>
+      <c r="E33">
+        <v>71</v>
+      </c>
+      <c r="F33">
+        <v>7.6</v>
+      </c>
+      <c r="G33" s="3">
+        <v>86</v>
+      </c>
+      <c r="H33" s="3">
+        <v>85</v>
+      </c>
+      <c r="I33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>162798565</v>
+      </c>
+      <c r="B34" s="3">
+        <v>291121</v>
+      </c>
+      <c r="C34" s="3">
+        <v>363258859</v>
+      </c>
+      <c r="D34" s="3">
+        <v>120000000</v>
+      </c>
+      <c r="E34" s="3">
+        <v>77</v>
+      </c>
+      <c r="F34" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="G34" s="3">
+        <v>92</v>
+      </c>
+      <c r="H34" s="3">
+        <v>72</v>
+      </c>
+      <c r="I34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>171091819</v>
+      </c>
+      <c r="B35" s="3">
+        <v>34221968</v>
+      </c>
+      <c r="C35" s="3">
+        <v>448191819</v>
+      </c>
+      <c r="D35" s="3">
+        <v>130000000</v>
+      </c>
+      <c r="E35">
+        <v>79</v>
+      </c>
+      <c r="F35">
+        <v>7.3</v>
+      </c>
+      <c r="G35" s="3">
+        <v>88</v>
+      </c>
+      <c r="H35" s="3">
+        <v>75</v>
+      </c>
+      <c r="I35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>137758063</v>
+      </c>
+      <c r="B36" s="3">
+        <v>38854851</v>
+      </c>
+      <c r="C36" s="3">
+        <v>349822765</v>
+      </c>
+      <c r="D36" s="3">
+        <v>127000000</v>
+      </c>
+      <c r="E36" s="3">
+        <v>56</v>
+      </c>
+      <c r="F36" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="G36" s="3">
+        <v>65</v>
+      </c>
+      <c r="H36" s="3">
+        <v>48</v>
+      </c>
+      <c r="I36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>144880014</v>
+      </c>
+      <c r="B37" s="3">
+        <v>2389226</v>
+      </c>
+      <c r="C37" s="3">
+        <v>216026182</v>
+      </c>
+      <c r="D37" s="3">
+        <v>4000000</v>
+      </c>
+      <c r="E37">
+        <v>83</v>
+      </c>
+      <c r="F37">
+        <v>7.2</v>
+      </c>
+      <c r="G37" s="3">
+        <v>98</v>
+      </c>
+      <c r="H37" s="3">
+        <v>76</v>
+      </c>
+      <c r="I37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>89302687</v>
+      </c>
+      <c r="B38" s="3">
+        <v>9812302</v>
+      </c>
+      <c r="C38" s="3">
+        <v>169327687</v>
+      </c>
+      <c r="D38" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="E38" s="3">
+        <v>70</v>
+      </c>
+      <c r="F38" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="G38" s="3">
+        <v>85</v>
+      </c>
+      <c r="H38" s="3">
+        <v>83</v>
+      </c>
+      <c r="I38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>289916256</v>
+      </c>
+      <c r="B39" s="3">
+        <v>62577067</v>
+      </c>
+      <c r="C39" s="3">
+        <v>630761313</v>
+      </c>
+      <c r="D39" s="3">
+        <v>115000000</v>
+      </c>
+      <c r="E39">
+        <v>78</v>
+      </c>
+      <c r="F39">
+        <v>8.1</v>
+      </c>
+      <c r="G39" s="3">
+        <v>96</v>
+      </c>
+      <c r="H39" s="3">
+        <v>90</v>
+      </c>
+      <c r="I39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>48430258</v>
+      </c>
+      <c r="B40" s="3">
+        <v>11889631</v>
+      </c>
+      <c r="C40" s="3">
+        <v>115121981</v>
+      </c>
+      <c r="D40" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="E40" s="3">
+        <v>49</v>
+      </c>
+      <c r="F40" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="G40" s="3">
+        <v>45</v>
+      </c>
+      <c r="H40" s="3">
+        <v>38</v>
+      </c>
+      <c r="I40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>145794338</v>
+      </c>
+      <c r="B41" s="3">
+        <v>35260212</v>
+      </c>
+      <c r="C41" s="3">
+        <v>273144151</v>
+      </c>
+      <c r="D41" s="3">
+        <v>80000000</v>
+      </c>
+      <c r="E41">
+        <v>73</v>
+      </c>
+      <c r="F41">
+        <v>7.2</v>
+      </c>
+      <c r="G41" s="3">
+        <v>86</v>
+      </c>
+      <c r="H41" s="3">
+        <v>77</v>
+      </c>
+      <c r="I41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>380843261</v>
+      </c>
+      <c r="B42" s="3">
+        <v>70251710</v>
+      </c>
+      <c r="C42" s="3">
+        <v>941615536</v>
+      </c>
+      <c r="D42" s="3">
+        <v>94000000</v>
+      </c>
+      <c r="E42" s="3">
+        <v>90</v>
+      </c>
+      <c r="F42" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="G42" s="3">
+        <v>99</v>
+      </c>
+      <c r="H42" s="3">
+        <v>86</v>
+      </c>
+      <c r="I42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>486295561</v>
+      </c>
+      <c r="B43" s="3">
+        <v>135060273</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1028570889</v>
+      </c>
+      <c r="D43" s="3">
+        <v>200000000</v>
+      </c>
+      <c r="E43">
+        <v>77</v>
+      </c>
+      <c r="F43">
+        <v>7.3</v>
+      </c>
+      <c r="G43" s="3">
+        <v>94</v>
+      </c>
+      <c r="H43" s="3">
+        <v>84</v>
+      </c>
+      <c r="I43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>85336277</v>
+      </c>
+      <c r="B44" s="3">
+        <v>291940</v>
+      </c>
+      <c r="C44" s="3">
+        <v>250397798</v>
+      </c>
+      <c r="D44" s="3">
+        <v>128000000</v>
+      </c>
+      <c r="E44" s="3">
+        <v>48</v>
+      </c>
+      <c r="F44" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="G44" s="3">
+        <v>37</v>
+      </c>
+      <c r="H44" s="3">
+        <v>64</v>
+      </c>
+      <c r="I44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>261441092</v>
+      </c>
+      <c r="B45" s="3">
+        <v>70467623</v>
+      </c>
+      <c r="C45" s="3">
+        <v>633184355</v>
+      </c>
+      <c r="D45" s="3">
+        <v>92000000</v>
+      </c>
+      <c r="E45">
+        <v>90</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45" s="3">
+        <v>97</v>
+      </c>
+      <c r="H45" s="3">
+        <v>75</v>
+      </c>
+      <c r="I45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>608581744</v>
+      </c>
+      <c r="B46" s="3">
+        <v>182687905</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1242805359</v>
+      </c>
+      <c r="D46" s="3">
+        <v>200000000</v>
+      </c>
+      <c r="E46" s="3">
+        <v>80</v>
+      </c>
+      <c r="F46" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="G46" s="3">
+        <v>94</v>
+      </c>
+      <c r="H46" s="3">
+        <v>85</v>
+      </c>
+      <c r="I46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>173008894</v>
+      </c>
+      <c r="B47" s="3">
+        <v>35142554</v>
+      </c>
+      <c r="C47" s="3">
+        <v>347512318</v>
+      </c>
+      <c r="D47" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="E47">
+        <v>39</v>
+      </c>
+      <c r="F47">
+        <v>6.9</v>
+      </c>
+      <c r="G47" s="3">
+        <v>45</v>
+      </c>
+      <c r="H47" s="3">
+        <v>76</v>
+      </c>
+      <c r="I47" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>